<commit_message>
new report bp v2
</commit_message>
<xml_diff>
--- a/web/excel/bp.xlsx
+++ b/web/excel/bp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\basic\web\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3D46863-3189-49B0-B63B-15D14E86361A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47B7620-BEE2-4C60-9C02-7FBD60F73B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>№</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>Регистрациялар сони</t>
-  </si>
-  <si>
-    <t>Жами</t>
   </si>
   <si>
     <t>Филиал</t>
@@ -384,12 +381,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -441,12 +437,6 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -552,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -586,28 +576,7 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,9 +608,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -986,10 +952,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1070,18 +1036,18 @@
     </row>
     <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+        <v>23</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+        <v>4</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="9"/>
       <c r="L4" s="10"/>
       <c r="M4" s="9"/>
@@ -1112,359 +1078,107 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="28" t="s">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="21" t="s">
+      <c r="Q6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="R6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="T6" s="21" t="s">
-        <v>23</v>
+      <c r="S6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-    </row>
-    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>1</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15">
-        <v>2000000</v>
-      </c>
-      <c r="D8" s="15">
-        <f>+C8*30%</f>
-        <v>600000</v>
-      </c>
-      <c r="E8" s="15">
-        <f>+C8+D8</f>
-        <v>2600000</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15">
-        <f>F8+G8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <f>+C8-F8</f>
-        <v>2000000</v>
-      </c>
-      <c r="J8" s="17">
-        <f>+F8/C8</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="15">
-        <f>+E8-H8</f>
-        <v>2600000</v>
-      </c>
-      <c r="L8" s="17">
-        <f>+G8/D8</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="15">
-        <f>+G8-J8</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="17">
-        <f>+H8/E8</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-    </row>
-    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
-        <f>1+A8</f>
-        <v>2</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-    </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <f t="shared" ref="A10:A15" si="0">1+A9</f>
-        <v>3</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-    </row>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-    </row>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-    </row>
-    <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-    </row>
-    <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-    </row>
-    <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="T6:T7"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="S6:S7"/>

</xml_diff>